<commit_message>
last modif to gather
</commit_message>
<xml_diff>
--- a/Evaluation_Results_Updated.xlsx
+++ b/Evaluation_Results_Updated.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
   </si>
   <si>
     <t>Precision</t>
@@ -407,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,185 +435,215 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0.85</v>
+      </c>
+      <c r="D2">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G2">
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0.85</v>
+      </c>
+      <c r="D3">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E3">
+        <v>0.5</v>
+      </c>
+      <c r="F3">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G3">
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.85</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.25</v>
+      </c>
+      <c r="F4">
+        <v>0.4</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0.95</v>
+      </c>
+      <c r="D5">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-      <c r="E2">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.8</v>
+      </c>
+      <c r="G5">
+        <v>0.9861111111111112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0.95</v>
+      </c>
+      <c r="D6">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.8</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.95</v>
+      </c>
+      <c r="D7">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.8</v>
+      </c>
+      <c r="G7">
+        <v>0.9722222222222222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>0.85</v>
+      </c>
+      <c r="D8">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="E8">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="F8">
+        <v>0.8695652173913043</v>
+      </c>
+      <c r="G8">
+        <v>0.8541666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>0.85</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.75</v>
+      </c>
+      <c r="F9">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G9">
+        <v>0.8645833333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>0.75</v>
+      </c>
+      <c r="D10">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="E10">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="F10">
+        <v>0.7619047619047619</v>
+      </c>
+      <c r="G10">
         <v>0.71875</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="E3">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F3">
-        <v>0.90625</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0.25</v>
-      </c>
-      <c r="E4">
-        <v>0.4</v>
-      </c>
-      <c r="F4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0.8</v>
-      </c>
-      <c r="F5">
-        <v>0.9861111111111112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.4444444444444444</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="D7">
-        <v>0.5</v>
-      </c>
-      <c r="E7">
-        <v>0.4</v>
-      </c>
-      <c r="F7">
-        <v>0.7361111111111112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>0.9090909090909091</v>
-      </c>
-      <c r="D8">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="E8">
-        <v>0.8695652173913043</v>
-      </c>
-      <c r="F8">
-        <v>0.8541666666666667</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0.75</v>
-      </c>
-      <c r="E9">
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="F9">
-        <v>0.8645833333333334</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="D10">
-        <v>0.75</v>
-      </c>
-      <c r="E10">
-        <v>0.6923076923076923</v>
-      </c>
-      <c r="F10">
-        <v>0.484375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>